<commit_message>
small updates to the guides
</commit_message>
<xml_diff>
--- a/Updated Guides/3 Excel Graphs Data.xlsx
+++ b/Updated Guides/3 Excel Graphs Data.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemissouristate-my.sharepoint.com/personal/eri2005_missouristate_edu/Documents/TEACHING/PSY-200/Updated Guides/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/TEACHING/PSY-200/Updated Guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{116F633F-7A00-114B-8E3F-1488B86442D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="10_ncr:8100000_{116F633F-7A00-114B-8E3F-1488B86442D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C6546F22-33F0-D14A-B933-FB0D7BB64147}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="2" xr2:uid="{48D4F59C-648B-ED4E-A5E4-EB152F2268C1}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{48D4F59C-648B-ED4E-A5E4-EB152F2268C1}"/>
   </bookViews>
   <sheets>
     <sheet name="One IV Bar" sheetId="1" r:id="rId1"/>
     <sheet name="Two IV Bar" sheetId="2" r:id="rId2"/>
     <sheet name="Scatter Plots" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Scatter Plots'!$A$2:$A$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Scatter Plots'!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Scatter Plots'!$B$2:$B$11</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -573,7 +568,487 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11281714785651793"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.86496062992125999"/>
+          <c:h val="0.78111840186643333"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Two IV Bar'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Men</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Two IV Bar'!$B$10:$C$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.75</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.35</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Two IV Bar'!$B$10:$C$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.75</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.35</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Two IV Bar'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No Cats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Owns Cats</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Two IV Bar'!$B$4:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C5B1-6C43-B82E-DE8A1DD55DF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Two IV Bar'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Women</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Two IV Bar'!$B$11:$C$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.8</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Two IV Bar'!$B$11:$C$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.8</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Two IV Bar'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No Cats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Owns Cats</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Two IV Bar'!$B$5:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C5B1-6C43-B82E-DE8A1DD55DF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1961797167"/>
+        <c:axId val="1956444367"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1961797167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cat Ownership</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1956444367"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1956444367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Rating of Cat Happiness</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1961797167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.25139741907261592"/>
+          <c:y val="5.1504082822980461E-2"/>
+          <c:w val="0.27964391951006123"/>
+          <c:h val="8.8667249927092448E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -587,23 +1062,84 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -631,15 +1167,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -649,15 +1185,51 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.44075546806649168"/>
+                  <c:y val="-3.0752405949256344E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -740,7 +1312,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-24EB-CA4B-8823-1EC439C3D8E9}"/>
+              <c16:uniqueId val="{00000000-39AD-FB48-95B1-6BEF04B802F9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -752,30 +1324,71 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="792594703"/>
-        <c:axId val="792512063"/>
+        <c:axId val="1991695583"/>
+        <c:axId val="1994951871"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="792594703"/>
+        <c:axId val="1991695583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Loves Dogs Rating</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -798,46 +1411,87 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="792512063"/>
+        <c:crossAx val="1994951871"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="792512063"/>
+        <c:axId val="1994951871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Loves Cats Rating</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -860,22 +1514,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="792594703"/>
+        <c:crossAx val="1991695583"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -918,7 +1572,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1200">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1011,6 +1668,12 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1515,6 +2178,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2035,15 +3201,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>654360</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>141114</xdr:rowOff>
+      <xdr:colOff>317261</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>70559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>261908</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>747957</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>24530</xdr:rowOff>
+      <xdr:rowOff>157802</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2075,23 +3241,64 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>657454</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>149302</xdr:rowOff>
+      <xdr:rowOff>158013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>263292</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>261719</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>30356</xdr:rowOff>
+      <xdr:rowOff>52484</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF15C73E-B263-044A-A0FC-082D2232D908}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA5EFE5-FCE2-A249-AE07-A6C019F57E12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>306658</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>56375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>758901</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>141868</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB5DD885-37E8-664B-A3B6-41D6AB78BD50}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2411,8 +3618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F211D117-FEF5-A645-8D33-62EA34FA522A}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2470,7 +3677,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A3" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2547,6 +3754,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2554,8 +3762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608DCBBD-0E2A-CA4A-923C-9CFC9437634F}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>